<commit_message>
[03-21] modified test scripts, added upload photos
</commit_message>
<xml_diff>
--- a/Carbids Tests Update.xlsx
+++ b/Carbids Tests Update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IA-Trainee\Documents\GitHub\Playwright-Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1728598C-1EFA-47CC-A185-659404954DBE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22885551-5106-4131-9FC7-D97F1E5DB767}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2520,7 +2520,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2539,6 +2539,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2552,7 +2558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2577,25 +2583,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2817,8 +2834,8 @@
   </sheetPr>
   <dimension ref="A1:X1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:E19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2875,28 +2892,28 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="12.75">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:24" ht="12.75">
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2906,11 +2923,11 @@
       <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="22" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2920,11 +2937,11 @@
       <c r="B5" s="1">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="5" t="s">
         <v>15</v>
       </c>
@@ -2934,11 +2951,11 @@
       <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="5" t="s">
         <v>17</v>
       </c>
@@ -2948,33 +2965,33 @@
       <c r="B7" s="1">
         <v>7</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:24" ht="12.75">
-      <c r="B8" s="19">
+      <c r="B8" s="14">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:24" ht="12.75">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +3002,7 @@
     </row>
     <row r="10" spans="1:24" ht="12.75">
       <c r="B10" s="1"/>
-      <c r="C10" s="17"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
         <v>24</v>
       </c>
@@ -2996,7 +3013,7 @@
     </row>
     <row r="11" spans="1:24" ht="12.75">
       <c r="B11" s="1"/>
-      <c r="C11" s="17"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="8" t="s">
         <v>26</v>
       </c>
@@ -3007,7 +3024,7 @@
     </row>
     <row r="12" spans="1:24" ht="12.75">
       <c r="B12" s="1"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="8" t="s">
         <v>28</v>
       </c>
@@ -3018,7 +3035,7 @@
     </row>
     <row r="13" spans="1:24" ht="12.75">
       <c r="B13" s="1"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="8" t="s">
         <v>30</v>
       </c>
@@ -3029,7 +3046,7 @@
     </row>
     <row r="14" spans="1:24" ht="12.75">
       <c r="B14" s="1"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="8" t="s">
         <v>32</v>
       </c>
@@ -3040,7 +3057,7 @@
     </row>
     <row r="15" spans="1:24" ht="12.75">
       <c r="B15" s="1"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="8" t="s">
         <v>34</v>
       </c>
@@ -3051,7 +3068,7 @@
     </row>
     <row r="16" spans="1:24" ht="12.75">
       <c r="B16" s="1"/>
-      <c r="C16" s="17"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="8" t="s">
         <v>36</v>
       </c>
@@ -3062,22 +3079,22 @@
     </row>
     <row r="17" spans="1:8" ht="12.75">
       <c r="B17" s="1"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="17"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:8" ht="12.75">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" ht="12.75">
       <c r="B19" s="1" t="s">
@@ -3086,10 +3103,10 @@
       <c r="C19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="5" t="s">
         <v>42</v>
       </c>
@@ -3102,10 +3119,10 @@
       <c r="C20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="5" t="s">
         <v>45</v>
       </c>
@@ -3118,10 +3135,10 @@
       <c r="C21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="5" t="s">
         <v>47</v>
       </c>
@@ -3137,7 +3154,7 @@
       <c r="D22" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="5" t="s">
         <v>50</v>
       </c>
@@ -3153,7 +3170,7 @@
       <c r="D23" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="5" t="s">
         <v>53</v>
       </c>
@@ -3166,10 +3183,10 @@
       <c r="C24" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="15"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="5" t="s">
         <v>55</v>
       </c>
@@ -3179,13 +3196,13 @@
       <c r="B25" s="1">
         <v>17</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="15"/>
+      <c r="E25" s="26"/>
       <c r="F25" s="5" t="s">
         <v>58</v>
       </c>
@@ -3195,13 +3212,13 @@
       <c r="B26" s="1">
         <v>18</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="5" t="s">
         <v>60</v>
       </c>
@@ -3211,41 +3228,41 @@
       <c r="B27" s="1">
         <v>19</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="15"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="5" t="s">
         <v>63</v>
       </c>
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:8" ht="12.75">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" ht="12.75">
       <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="15"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="5" t="s">
         <v>67</v>
       </c>
@@ -3255,13 +3272,13 @@
       <c r="B30" s="1">
         <v>23</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="26"/>
       <c r="F30" s="5" t="s">
         <v>69</v>
       </c>
@@ -3271,13 +3288,13 @@
       <c r="B31" s="1">
         <v>24</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="15"/>
+      <c r="E31" s="26"/>
       <c r="F31" s="5" t="s">
         <v>72</v>
       </c>
@@ -3287,13 +3304,13 @@
       <c r="B32" s="1">
         <v>25</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="5" t="s">
         <v>74</v>
       </c>
@@ -3303,13 +3320,13 @@
       <c r="B33" s="1">
         <v>26</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="15"/>
+      <c r="E33" s="26"/>
       <c r="F33" s="5" t="s">
         <v>76</v>
       </c>
@@ -3319,13 +3336,13 @@
       <c r="B34" s="1">
         <v>27</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="26"/>
       <c r="F34" s="5" t="s">
         <v>79</v>
       </c>
@@ -3335,13 +3352,13 @@
       <c r="B35" s="1">
         <v>28</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="26"/>
       <c r="F35" s="5" t="s">
         <v>81</v>
       </c>
@@ -10202,12 +10219,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="A18:H18"/>
@@ -10218,21 +10244,12 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C7:C17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C3:C6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G7 G19:G27 G29:G35" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>